<commit_message>
Unit configurations; Scenario 8 story and concept; scenario 1 - 7 balancing; added real-life photographs to potentially replace AI-generated story backgrounds in the future
</commit_message>
<xml_diff>
--- a/units/Kalgor/Damage.xlsx
+++ b/units/Kalgor/Damage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c009ef319659ad0f/Dokumente/My Games/Wesnoth1.16/data/add-ons/deception/units/Kalgor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="457" documentId="11_F25DC773A252ABDACC1048AA191E4DF65BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0639DAC-A941-4637-879F-A451132ADEBC}"/>
+  <xr:revisionPtr revIDLastSave="497" documentId="11_F25DC773A252ABDACC1048AA191E4DF65BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB7496D2-D588-41E6-B566-883C1AD116EB}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="17472" windowHeight="10992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="19386" windowHeight="12186" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -441,21 +441,21 @@
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <selection activeCell="C5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="2" width="6.578125" customWidth="1"/>
-    <col min="3" max="3" width="14.578125" customWidth="1"/>
-    <col min="4" max="6" width="6.1015625" style="1" customWidth="1"/>
-    <col min="7" max="9" width="6.1015625" style="2" customWidth="1"/>
-    <col min="10" max="12" width="6.1015625" style="1" customWidth="1"/>
-    <col min="13" max="15" width="6.1015625" style="2" customWidth="1"/>
-    <col min="16" max="18" width="6.1015625" style="3" customWidth="1"/>
+    <col min="1" max="2" width="6.5859375" customWidth="1"/>
+    <col min="3" max="3" width="14.5859375" customWidth="1"/>
+    <col min="4" max="6" width="6.1171875" style="1" customWidth="1"/>
+    <col min="7" max="9" width="6.1171875" style="2" customWidth="1"/>
+    <col min="10" max="12" width="6.1171875" style="1" customWidth="1"/>
+    <col min="13" max="15" width="6.1171875" style="2" customWidth="1"/>
+    <col min="16" max="18" width="6.1171875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -488,7 +488,7 @@
       <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -499,34 +499,34 @@
         <v>7</v>
       </c>
       <c r="D2" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1">
         <v>2</v>
       </c>
       <c r="F2" s="1">
         <f>D2*E2</f>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G2" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H2" s="2">
         <v>4</v>
       </c>
       <c r="I2" s="2">
         <f>G2*H2</f>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="J2" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K2" s="1">
         <v>3</v>
       </c>
       <c r="L2" s="1">
         <f>J2*K2</f>
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="M2" s="2">
         <v>7</v>
@@ -549,7 +549,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -560,44 +560,44 @@
         <v>8</v>
       </c>
       <c r="D3" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
       </c>
       <c r="F3" s="1">
         <f t="shared" ref="F3:F7" si="0">D3*E3</f>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G3" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H3" s="2">
         <v>4</v>
       </c>
       <c r="I3" s="2">
         <f t="shared" ref="I3:I7" si="1">G3*H3</f>
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J3" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K3" s="1">
         <v>3</v>
       </c>
       <c r="L3" s="1">
         <f t="shared" ref="L3:L7" si="2">J3*K3</f>
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="M3" s="2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="N3" s="2">
         <v>2</v>
       </c>
       <c r="O3" s="2">
         <f t="shared" ref="O3:O9" si="3">M3*N3</f>
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="P3" s="3">
         <v>9</v>
@@ -606,11 +606,11 @@
         <v>3</v>
       </c>
       <c r="R3" s="3">
-        <f t="shared" ref="R3:R9" si="4">P3*Q3</f>
+        <f t="shared" ref="R3:R7" si="4">P3*Q3</f>
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -621,44 +621,44 @@
         <v>9</v>
       </c>
       <c r="D4" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" ref="F4" si="5">D4*E4</f>
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G4" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H4" s="2">
         <v>4</v>
       </c>
       <c r="I4" s="2">
         <f t="shared" ref="I4" si="6">G4*H4</f>
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="J4" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K4" s="1">
         <v>3</v>
       </c>
       <c r="L4" s="1">
         <f t="shared" ref="L4" si="7">J4*K4</f>
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M4" s="2">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="N4" s="2">
         <v>2</v>
       </c>
       <c r="O4" s="2">
         <f t="shared" ref="O4" si="8">M4*N4</f>
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="P4" s="3">
         <v>12</v>
@@ -671,7 +671,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -682,44 +682,44 @@
         <v>10</v>
       </c>
       <c r="D5" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="1">
         <v>2</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G5" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H5" s="2">
         <v>4</v>
       </c>
       <c r="I5" s="2">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J5" s="1">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K5" s="1">
         <v>3</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" si="2"/>
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="M5" s="2">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="N5" s="2">
         <v>2</v>
       </c>
       <c r="O5" s="2">
         <f t="shared" si="3"/>
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="P5" s="3">
         <v>14</v>
@@ -732,49 +732,49 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.5">
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="1">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E6" s="1">
         <v>2</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G6" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H6" s="2">
         <v>4</v>
       </c>
       <c r="I6" s="2">
         <f t="shared" si="1"/>
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="J6" s="1">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K6" s="1">
         <v>3</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="M6" s="2">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="N6" s="2">
         <v>2</v>
       </c>
       <c r="O6" s="2">
         <f t="shared" si="3"/>
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="P6" s="3">
         <v>16</v>
@@ -787,49 +787,49 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.5">
       <c r="C7" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="1">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E7" s="1">
         <v>2</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G7" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H7" s="2">
         <v>4</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="J7" s="1">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K7" s="1">
         <v>3</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" si="2"/>
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="M7" s="2">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N7" s="2">
         <v>2</v>
       </c>
       <c r="O7" s="2">
         <f t="shared" si="3"/>
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="P7" s="3">
         <v>17</v>
@@ -842,64 +842,64 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.5">
       <c r="C8" t="s">
         <v>13</v>
       </c>
       <c r="M8" s="2">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="N8" s="2">
         <v>3</v>
       </c>
       <c r="O8" s="2">
         <f t="shared" si="3"/>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.5">
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="M9" s="2">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="N9" s="2">
         <v>4</v>
       </c>
       <c r="O9" s="2">
         <f t="shared" si="3"/>
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.5">
       <c r="C10" t="s">
         <v>15</v>
       </c>
       <c r="P10" s="3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q10" s="3">
         <v>4</v>
       </c>
       <c r="R10" s="3">
         <f>P10*Q10</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.5">
       <c r="C11" t="s">
         <v>16</v>
       </c>
       <c r="P11" s="3">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q11" s="3">
         <v>5</v>
       </c>
       <c r="R11" s="3">
         <f>P11*Q11</f>
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Elvish Stormfeather improved and added animation sprites; Elvish Paragon improvement to further distinguish from Elvish Marshal; Removed Orcish Boltstorm (had copied from LotI), with Orcish Dreadbolt the only remaining Slurbow lvl 4 advancement; Adjusted level 3 units with custom level 4 advancements to have a more linear XP progression from level 1>2>3>4; Kalgor advances to max level 3, reducing his max power, and receives a 20% XP increase per level up; Unit image structure: Every unit has their own sub-directory within its race folder; Added new weapon special 'scourge' to Orcish Bloodscourge, Orcish Doombringer and Banescourge
</commit_message>
<xml_diff>
--- a/units/Kalgor/Damage.xlsx
+++ b/units/Kalgor/Damage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c009ef319659ad0f/Dokumente/My Games/Wesnoth1.16/data/add-ons/deception/units/Kalgor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="497" documentId="11_F25DC773A252ABDACC1048AA191E4DF65BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB7496D2-D588-41E6-B566-883C1AD116EB}"/>
+  <xr:revisionPtr revIDLastSave="518" documentId="11_F25DC773A252ABDACC1048AA191E4DF65BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5503F1B1-8589-40B0-9170-38C875047663}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="19386" windowHeight="12186" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22046" yWindow="-103" windowWidth="22149" windowHeight="12549" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Type</t>
   </si>
@@ -68,25 +68,16 @@
     <t>level 3</t>
   </si>
   <si>
-    <t>level 4</t>
-  </si>
-  <si>
     <t>strength 1</t>
   </si>
   <si>
     <t>strength 2</t>
   </si>
   <si>
-    <t>abyss 1</t>
-  </si>
-  <si>
-    <t>abyss 2</t>
-  </si>
-  <si>
-    <t>darkness 1</t>
-  </si>
-  <si>
-    <t>darkness 2</t>
+    <t>abyss</t>
+  </si>
+  <si>
+    <t>darkness</t>
   </si>
 </sst>
 </file>
@@ -438,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C5" sqref="A5:XFD5"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -566,7 +557,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F7" si="0">D3*E3</f>
+        <f t="shared" ref="F3:F6" si="0">D3*E3</f>
         <v>28</v>
       </c>
       <c r="G3" s="2">
@@ -576,7 +567,7 @@
         <v>4</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" ref="I3:I7" si="1">G3*H3</f>
+        <f t="shared" ref="I3:I6" si="1">G3*H3</f>
         <v>32</v>
       </c>
       <c r="J3" s="1">
@@ -586,7 +577,7 @@
         <v>3</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L7" si="2">J3*K3</f>
+        <f t="shared" ref="L3:L6" si="2">J3*K3</f>
         <v>36</v>
       </c>
       <c r="M3" s="2">
@@ -596,7 +587,7 @@
         <v>2</v>
       </c>
       <c r="O3" s="2">
-        <f t="shared" ref="O3:O9" si="3">M3*N3</f>
+        <f t="shared" ref="O3:O7" si="3">M3*N3</f>
         <v>18</v>
       </c>
       <c r="P3" s="3">
@@ -672,44 +663,38 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.5">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="1">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1">
         <v>2</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G5" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H5" s="2">
         <v>4</v>
       </c>
       <c r="I5" s="2">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="J5" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K5" s="1">
         <v>3</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="M5" s="2">
         <v>13</v>
@@ -737,34 +722,34 @@
         <v>11</v>
       </c>
       <c r="D6" s="1">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1">
         <v>2</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G6" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H6" s="2">
         <v>4</v>
       </c>
       <c r="I6" s="2">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J6" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K6" s="1">
         <v>3</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="2"/>
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M6" s="2">
         <v>15</v>
@@ -777,129 +762,44 @@
         <v>30</v>
       </c>
       <c r="P6" s="3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q6" s="3">
         <v>3</v>
       </c>
       <c r="R6" s="3">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.5">
       <c r="C7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="1">
-        <v>23</v>
-      </c>
-      <c r="E7" s="1">
-        <v>2</v>
-      </c>
-      <c r="F7" s="1">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="G7" s="2">
-        <v>14</v>
-      </c>
-      <c r="H7" s="2">
-        <v>4</v>
-      </c>
-      <c r="I7" s="2">
-        <f t="shared" si="1"/>
-        <v>56</v>
-      </c>
-      <c r="J7" s="1">
-        <v>19</v>
-      </c>
-      <c r="K7" s="1">
-        <v>3</v>
-      </c>
-      <c r="L7" s="1">
-        <f t="shared" si="2"/>
-        <v>57</v>
-      </c>
       <c r="M7" s="2">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="N7" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O7" s="2">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P7" s="3">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="Q7" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R7" s="3">
         <f t="shared" si="4"/>
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.5">
       <c r="C8" t="s">
         <v>13</v>
-      </c>
-      <c r="M8" s="2">
-        <v>13</v>
-      </c>
-      <c r="N8" s="2">
-        <v>3</v>
-      </c>
-      <c r="O8" s="2">
-        <f t="shared" si="3"/>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.5">
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="M9" s="2">
-        <v>11</v>
-      </c>
-      <c r="N9" s="2">
-        <v>4</v>
-      </c>
-      <c r="O9" s="2">
-        <f t="shared" si="3"/>
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.5">
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-      <c r="P10" s="3">
-        <v>14</v>
-      </c>
-      <c r="Q10" s="3">
-        <v>4</v>
-      </c>
-      <c r="R10" s="3">
-        <f>P10*Q10</f>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.5">
-      <c r="C11" t="s">
-        <v>16</v>
-      </c>
-      <c r="P11" s="3">
-        <v>12</v>
-      </c>
-      <c r="Q11" s="3">
-        <v>5</v>
-      </c>
-      <c r="R11" s="3">
-        <f>P11*Q11</f>
-        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>